<commit_message>
MOSFET Chip 2x3 Panel RTM.
</commit_message>
<xml_diff>
--- a/mosfet-chip/panelized/fab runs/mosfet_chip-v1_0-2022-06-05/mosfet_chip-v1_0-2022-06-05-JLCSMT-BOM.xlsx
+++ b/mosfet-chip/panelized/fab runs/mosfet_chip-v1_0-2022-06-05/mosfet_chip-v1_0-2022-06-05-JLCSMT-BOM.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\like-the-art\mosfet-chip\fab runs\mosfet_chip-v1_0-2022-06-05\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akimb\Documents\PCB CAD Projects\like-the-art\mosfet-chip\panelized\fab runs\mosfet_chip-v1_0-2022-06-05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9988361C-21D2-4B42-874C-D2644A43D5BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2751D0D8-566F-4ABA-AB1A-69CE613B0DD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3816" yWindow="1764" windowWidth="22416" windowHeight="13368" xr2:uid="{B073D8ED-5E93-4247-85AA-3657D4BF98F8}"/>
+    <workbookView xWindow="3072" yWindow="972" windowWidth="22416" windowHeight="13368" xr2:uid="{B073D8ED-5E93-4247-85AA-3657D4BF98F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>XL-1608SURC-06</t>
   </si>
   <si>
-    <t>LED_SMD:LED_0603_1608Metric</t>
-  </si>
-  <si>
     <t>C965799</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Phoenix Contact</t>
   </si>
   <si>
-    <t>Package_TO_SOT_THT:TO-220-3_Vertical</t>
-  </si>
-  <si>
     <t>C513144</t>
   </si>
   <si>
@@ -68,9 +62,6 @@
     <t>IRLZ34NPbF</t>
   </si>
   <si>
-    <t>Resistor_SMD:R_0603_1608Metric</t>
-  </si>
-  <si>
     <t xml:space="preserve">10K 1% 1/10W </t>
   </si>
   <si>
@@ -144,6 +135,12 @@
   </si>
   <si>
     <t>0603WAF3301T5E</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>TO-220-3</t>
   </si>
 </sst>
 </file>
@@ -187,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -202,6 +199,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -522,183 +520,186 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F5" sqref="F5:F7"/>
+      <selection pane="bottomRight" activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="3"/>
+    <col min="7" max="7" width="4" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
       </c>
       <c r="F3" s="5">
         <v>1711725</v>
       </c>
       <c r="G3" s="3">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" t="s">
+      <c r="F4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>10</v>
-      </c>
       <c r="G4" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>34</v>
-      </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>11</v>
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E6" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="G6" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>11</v>
+        <v>24</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>34</v>
       </c>
       <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
       <c r="G7" s="3">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="C2:C7" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>